<commit_message>
Feat: Update table info
</commit_message>
<xml_diff>
--- a/2. Analysis/2. Database/table_info.xlsx
+++ b/2. Analysis/2. Database/table_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xcg32\OneDrive\DOCUME~1-LAPTOP-6KVPMOUI-1300945\2. 개발\1. 해외축구 분석\FooballAnalytics\2. Analysis\2. Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xcg32\OneDrive\DOCUME~1-LAPTOP-6KVPMOUI-1300945\3. 개발\1. 해외축구 분석\FooballAnalytics\2. Analysis\2. Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27082F10-91FF-4C34-B818-F738E3AE40D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4AE526-F741-4DC5-926E-DE596FCE1445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{F146DD27-610E-4900-9E27-3DE9F447F969}"/>
+    <workbookView xWindow="135" yWindow="1215" windowWidth="21600" windowHeight="11295" xr2:uid="{F146DD27-610E-4900-9E27-3DE9F447F969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
   <si>
     <t>England</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,6 +135,162 @@
   </si>
   <si>
     <t>captain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arteta</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Odegard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Son</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>won</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drawn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ga</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yellow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tbl_season_position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chelsea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Man CIty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tbl_season_match</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>round</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>referee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>opp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>last5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fhgf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fhga</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shgf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shga</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shot_on_target</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foul</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>acc_point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>acc_gd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>acc_gf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timestamp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>integer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -159,7 +315,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +334,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -193,7 +355,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -201,6 +363,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -517,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E437755C-4070-4524-93B4-790CE02BDB55}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -529,12 +694,12 @@
     <col min="3" max="3" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -542,118 +707,455 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>74310</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB31" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="S32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB32" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>